<commit_message>
Auto update 2025-09-03 10:52:44
</commit_message>
<xml_diff>
--- a/data/eeee.xlsx
+++ b/data/eeee.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\BPL_Dashboard\architecture_based\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aishwarrya VP\OneDrive - BPL Medical Technologies Pvt. Ltd\Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>Task</t>
   </si>
@@ -202,6 +202,21 @@
   </si>
   <si>
     <t>Not Started</t>
+  </si>
+  <si>
+    <t>2025-10-04</t>
+  </si>
+  <si>
+    <t>2025-08-23</t>
+  </si>
+  <si>
+    <t>Reframe the requirements of C VIEW-FD</t>
+  </si>
+  <si>
+    <t>Make the new SRS for CVIEW-FD</t>
+  </si>
+  <si>
+    <t>Aishwarrya VP;Thakarkuldip</t>
   </si>
 </sst>
 </file>
@@ -754,8 +769,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H22" totalsRowShown="0">
-  <autoFilter ref="A1:H22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H24" totalsRowShown="0">
+  <autoFilter ref="A1:H24"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Task No"/>
     <tableColumn id="2" name="Task"/>
@@ -1033,25 +1048,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.36328125" customWidth="1"/>
-    <col min="2" max="2" width="68.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.90625" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="34.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -1077,7 +1092,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1103,7 +1118,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1126,7 +1141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1149,7 +1164,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1172,7 +1187,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1195,7 +1210,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1218,7 +1233,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1241,7 +1256,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1264,7 +1279,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1287,7 +1302,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1310,7 +1325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1333,7 +1348,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1356,7 +1371,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1379,7 +1394,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1402,7 +1417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1425,7 +1440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1448,7 +1463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1471,7 +1486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1494,7 +1509,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1517,7 +1532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1540,7 +1555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1560,6 +1575,52 @@
         <v>55</v>
       </c>
       <c r="G22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23">
+        <v>25</v>
+      </c>
+      <c r="E23" s="1">
+        <v>45793</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>45859</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update 2025-09-03 11:10:05
</commit_message>
<xml_diff>
--- a/data/eeee.xlsx
+++ b/data/eeee.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
   <si>
     <t>Task</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>Aishwarrya VP;Thakarkuldip</t>
+  </si>
+  <si>
+    <t>2025-08-24</t>
+  </si>
+  <si>
+    <t>Submit the SRS</t>
   </si>
 </sst>
 </file>
@@ -769,8 +775,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H24" totalsRowShown="0">
-  <autoFilter ref="A1:H24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H25" totalsRowShown="0">
+  <autoFilter ref="A1:H25"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Task No"/>
     <tableColumn id="2" name="Task"/>
@@ -1048,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,6 +1630,29 @@
         <v>20</v>
       </c>
     </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>45860</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Auto update changes 2025-09-03 12:33:51
</commit_message>
<xml_diff>
--- a/data/eeee.xlsx
+++ b/data/eeee.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
   <si>
     <t>Task</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>Submit the SRS</t>
+  </si>
+  <si>
+    <t>2025-08-25</t>
+  </si>
+  <si>
+    <t>Get approval</t>
   </si>
 </sst>
 </file>
@@ -775,8 +781,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H25" totalsRowShown="0">
-  <autoFilter ref="A1:H25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H26" totalsRowShown="0">
+  <autoFilter ref="A1:H26"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Task No"/>
     <tableColumn id="2" name="Task"/>
@@ -1054,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1650,7 +1656,30 @@
         <v>66</v>
       </c>
       <c r="G25" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>45861</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update changes 2025-09-03 12:37:45
</commit_message>
<xml_diff>
--- a/data/eeee.xlsx
+++ b/data/eeee.xlsx
@@ -228,7 +228,7 @@
     <t>2025-08-25</t>
   </si>
   <si>
-    <t>Get approval</t>
+    <t>Get approval from sales/DQA</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Auto update changes 2025-09-03 12:41:23
</commit_message>
<xml_diff>
--- a/data/eeee.xlsx
+++ b/data/eeee.xlsx
@@ -222,13 +222,13 @@
     <t>2025-08-24</t>
   </si>
   <si>
-    <t>Submit the SRS</t>
-  </si>
-  <si>
     <t>2025-08-25</t>
   </si>
   <si>
     <t>Get approval from sales/DQA</t>
+  </si>
+  <si>
+    <t>Submit the SRS to DQA</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,7 +1641,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
         <v>60</v>
@@ -1664,7 +1664,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
         <v>60</v>
@@ -1676,7 +1676,7 @@
         <v>45861</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G26" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Auto update 2025-09-03 13:47:06
</commit_message>
<xml_diff>
--- a/data/eeee.xlsx
+++ b/data/eeee.xlsx
@@ -1,241 +1,231 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aishwarrya VP\OneDrive - BPL Medical Technologies Pvt. Ltd\Exports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\BPL_Dashboard\architecture_based\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_87A7B570DA54221654195706922A35277DE99C6F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updateddata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
+  <si>
+    <t>Task No</t>
+  </si>
   <si>
     <t>Task</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>End date</t>
+  </si>
+  <si>
     <t>Assignees</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Progress</t>
-  </si>
-  <si>
-    <t>Start date</t>
-  </si>
-  <si>
-    <t>End date</t>
+    <t>Remarks</t>
   </si>
   <si>
     <t>Multi Export to be added from C View II to C View FD</t>
   </si>
   <si>
+    <t>Not Started</t>
+  </si>
+  <si>
     <t>Aishwarrya VP;Vrinda Bhat</t>
   </si>
   <si>
+    <t>Dependecy issue, less information</t>
+  </si>
+  <si>
     <t>Pan bug - Export screen</t>
   </si>
   <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>2025-10-15</t>
+  </si>
+  <si>
     <t>Thakarkuldip;Aishwarrya VP;Vrinda Bhat</t>
   </si>
   <si>
     <t>Remove FPS and drop down and Add Speed</t>
   </si>
   <si>
+    <t>Hold</t>
+  </si>
+  <si>
+    <t>2025-10-27</t>
+  </si>
+  <si>
     <t>Vrinda Bhat</t>
   </si>
   <si>
     <t>Clean Cview FD code, remove the warnings</t>
   </si>
   <si>
+    <t>2025-08-27</t>
+  </si>
+  <si>
     <t>Thakarkuldip;Vrinda Bhat</t>
   </si>
   <si>
     <t>Setup Code structure for release and Debug configuration</t>
   </si>
   <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>2025-08-19</t>
+  </si>
+  <si>
     <t>Thakarkuldip</t>
   </si>
   <si>
     <t>R&amp;D for SharpScan (Image quality check software)</t>
   </si>
   <si>
-    <t>In Progress</t>
+    <t>2025-07-25</t>
   </si>
   <si>
     <t>Checking FFT transform for image with different filter , to resolve grid lines issue</t>
   </si>
   <si>
+    <t>2025-08-14</t>
+  </si>
+  <si>
     <t>Set default x64 release architecture for Cview-FD code.</t>
   </si>
   <si>
+    <t>2025-08-09</t>
+  </si>
+  <si>
     <t>Aishwarrya VP</t>
   </si>
   <si>
     <t>Merge all the changes to one final updated code</t>
   </si>
   <si>
+    <t>2025-09-01</t>
+  </si>
+  <si>
     <t>Dynamically change the UI of the Splash screen</t>
   </si>
   <si>
+    <t>2025-07-11</t>
+  </si>
+  <si>
     <t>Enable and Disable buttons during Exposure</t>
   </si>
   <si>
+    <t>2025-09-06</t>
+  </si>
+  <si>
     <t>Offset status bar</t>
   </si>
   <si>
+    <t>2025-06-29</t>
+  </si>
+  <si>
     <t>Hardware Settings - Save clicked - closes application</t>
   </si>
   <si>
+    <t>2025-06-30</t>
+  </si>
+  <si>
     <t>Worklist gets hanged - during reconnection</t>
   </si>
   <si>
+    <t>2025-07-09</t>
+  </si>
+  <si>
     <t>Add to Ref button - added in Recall Section</t>
   </si>
   <si>
+    <t>2025-10-28</t>
+  </si>
+  <si>
     <t>Collect Multiple good and bad images to train model For R&amp;D</t>
   </si>
   <si>
+    <t>2025-11-19</t>
+  </si>
+  <si>
+    <t>Collect images and write Custom algorithm to Enhance the image quality</t>
+  </si>
+  <si>
+    <t>2025-09-17</t>
+  </si>
+  <si>
+    <t>Explore about DSA to implement for Cview FD</t>
+  </si>
+  <si>
+    <t>2025-11-15</t>
+  </si>
+  <si>
+    <t>Start implementing OPENCV in the current code to optimize and increase speed.</t>
+  </si>
+  <si>
     <t>In plan</t>
   </si>
   <si>
-    <t>Collect images and write Custom algorithm to Enhance the image quality</t>
-  </si>
-  <si>
-    <t>Explore about DSA to implement for Cview FD</t>
-  </si>
-  <si>
-    <t>Start implementing OPENCV in the current code to optimize and increase speed.</t>
+    <t>2025-06-20</t>
   </si>
   <si>
     <t>Find a suitable way to reduce the time taken for software initialization.</t>
   </si>
   <si>
+    <t>2025-10-03</t>
+  </si>
+  <si>
     <t>Get DSA Code of XMED from Niha's PC</t>
   </si>
   <si>
-    <t>Task No</t>
-  </si>
-  <si>
-    <t>2025-09-01</t>
-  </si>
-  <si>
-    <t>2025-10-15</t>
-  </si>
-  <si>
-    <t>2025-10-27</t>
-  </si>
-  <si>
-    <t>2025-08-27</t>
-  </si>
-  <si>
-    <t>2025-08-19</t>
-  </si>
-  <si>
-    <t>2025-07-25</t>
-  </si>
-  <si>
-    <t>2025-08-14</t>
-  </si>
-  <si>
-    <t>2025-08-09</t>
-  </si>
-  <si>
-    <t>2025-07-11</t>
-  </si>
-  <si>
-    <t>2025-09-06</t>
-  </si>
-  <si>
-    <t>2025-06-29</t>
-  </si>
-  <si>
-    <t>2025-06-30</t>
-  </si>
-  <si>
-    <t>2025-07-09</t>
-  </si>
-  <si>
-    <t>2025-10-28</t>
-  </si>
-  <si>
-    <t>2025-11-19</t>
-  </si>
-  <si>
-    <t>2025-09-17</t>
-  </si>
-  <si>
-    <t>2025-11-15</t>
-  </si>
-  <si>
-    <t>2025-06-20</t>
-  </si>
-  <si>
-    <t>2025-10-03</t>
-  </si>
-  <si>
     <t>2025-08-22</t>
-  </si>
-  <si>
-    <t>Hold</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>Dependecy issue, less information</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>Not Started</t>
-  </si>
-  <si>
-    <t>2025-10-04</t>
-  </si>
-  <si>
-    <t>2025-08-23</t>
-  </si>
-  <si>
-    <t>Reframe the requirements of C VIEW-FD</t>
-  </si>
-  <si>
-    <t>Make the new SRS for CVIEW-FD</t>
-  </si>
-  <si>
-    <t>Aishwarrya VP;Thakarkuldip</t>
-  </si>
-  <si>
-    <t>2025-08-24</t>
-  </si>
-  <si>
-    <t>2025-08-25</t>
-  </si>
-  <si>
-    <t>Get approval from sales/DQA</t>
-  </si>
-  <si>
-    <t>Submit the SRS to DQA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -762,10 +752,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -781,17 +771,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H26" totalsRowShown="0">
-  <autoFilter ref="A1:H26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:H22" totalsRowShown="0">
+  <autoFilter ref="A1:H22" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Task No"/>
-    <tableColumn id="2" name="Task"/>
-    <tableColumn id="3" name="Status"/>
-    <tableColumn id="4" name="Progress"/>
-    <tableColumn id="5" name="Start date" dataDxfId="1"/>
-    <tableColumn id="6" name="End date" dataDxfId="0"/>
-    <tableColumn id="7" name="Assignees"/>
-    <tableColumn id="8" name="Remarks"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start date" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="End date" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Assignees"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Remarks"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1059,14 +1049,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="68.140625" bestFit="1" customWidth="1"/>
@@ -1078,12 +1068,12 @@
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1098,21 +1088,21 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1124,21 +1114,21 @@
         <v>45818</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>100</v>
@@ -1147,21 +1137,21 @@
         <v>45755</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>25</v>
@@ -1170,21 +1160,21 @@
         <v>45777</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>75</v>
@@ -1193,21 +1183,21 @@
         <v>45670</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -1216,21 +1206,21 @@
         <v>45779</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <v>25</v>
@@ -1239,21 +1229,21 @@
         <v>45738</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>100</v>
@@ -1262,21 +1252,21 @@
         <v>45767</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -1285,21 +1275,21 @@
         <v>45799</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>100</v>
@@ -1308,21 +1298,21 @@
         <v>45731</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>25</v>
@@ -1331,21 +1321,21 @@
         <v>45790</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D12">
         <v>50</v>
@@ -1354,21 +1344,21 @@
         <v>45702</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
       </c>
       <c r="D13">
         <v>25</v>
@@ -1377,21 +1367,21 @@
         <v>45707</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D14">
         <v>75</v>
@@ -1400,21 +1390,21 @@
         <v>45665</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D15">
         <v>50</v>
@@ -1423,21 +1413,21 @@
         <v>45758</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D16">
         <v>25</v>
@@ -1446,21 +1436,21 @@
         <v>45672</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1469,21 +1459,21 @@
         <v>45698</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D18">
         <v>25</v>
@@ -1495,18 +1485,18 @@
         <v>51</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="D19">
         <v>100</v>
@@ -1515,21 +1505,21 @@
         <v>45675</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="D20">
         <v>25</v>
@@ -1538,21 +1528,21 @@
         <v>45807</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1561,21 +1551,21 @@
         <v>45661</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="D22">
         <v>100</v>
@@ -1584,102 +1574,10 @@
         <v>45727</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23">
-        <v>25</v>
-      </c>
-      <c r="E23" s="1">
-        <v>45793</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1">
-        <v>45859</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1">
-        <v>45860</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1">
-        <v>45861</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G26" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update 2025-09-03 13:52:30
</commit_message>
<xml_diff>
--- a/data/eeee.xlsx
+++ b/data/eeee.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29225"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\BPL_Dashboard\architecture_based\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive - BPL Medical Technologies Pvt. Ltd\Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_87A7B570DA54221654195706922A35277DE99C6F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="updateddata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <t>Task No</t>
   </si>
@@ -219,13 +218,16 @@
   </si>
   <si>
     <t>2025-08-22</t>
+  </si>
+  <si>
+    <t>Get DSA Code of XMED from Niha's PC vah vah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -752,10 +754,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -771,17 +773,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:H22" totalsRowShown="0">
-  <autoFilter ref="A1:H22" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H23" totalsRowShown="0">
+  <autoFilter ref="A1:H23"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task No"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start date" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="End date" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Assignees"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Remarks"/>
+    <tableColumn id="1" name="Task No"/>
+    <tableColumn id="2" name="Task"/>
+    <tableColumn id="3" name="Status"/>
+    <tableColumn id="4" name="Progress"/>
+    <tableColumn id="5" name="Start date" dataDxfId="1"/>
+    <tableColumn id="6" name="End date" dataDxfId="0"/>
+    <tableColumn id="7" name="Assignees"/>
+    <tableColumn id="8" name="Remarks"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1049,26 +1051,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="68.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1120,7 +1122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1143,7 +1145,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1166,7 +1168,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1189,7 +1191,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1212,7 +1214,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1235,7 +1237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1258,7 +1260,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1281,7 +1283,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1304,7 +1306,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1327,7 +1329,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1350,7 +1352,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1373,7 +1375,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1396,7 +1398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1419,7 +1421,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1442,7 +1444,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1465,7 +1467,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1488,7 +1490,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1511,7 +1513,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1534,7 +1536,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1557,7 +1559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1577,6 +1579,29 @@
         <v>60</v>
       </c>
       <c r="G22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>100</v>
+      </c>
+      <c r="E23" s="1">
+        <v>45727</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update 2025-09-03 13:54:04
</commit_message>
<xml_diff>
--- a/data/eeee.xlsx
+++ b/data/eeee.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t>Task No</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>Get DSA Code of XMED from Niha's PC vah vah</t>
+  </si>
+  <si>
+    <t>Get DSA Code of XMED from Niha's PC vah vah vah3</t>
   </si>
 </sst>
 </file>
@@ -773,8 +776,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H23" totalsRowShown="0">
-  <autoFilter ref="A1:H23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H24" totalsRowShown="0">
+  <autoFilter ref="A1:H24"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Task No"/>
     <tableColumn id="2" name="Task"/>
@@ -1052,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1605,6 +1608,29 @@
         <v>33</v>
       </c>
     </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24">
+        <v>100</v>
+      </c>
+      <c r="E24" s="1">
+        <v>45727</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Auto update 2025-09-03 13:58:10
</commit_message>
<xml_diff>
--- a/data/eeee.xlsx
+++ b/data/eeee.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
   <si>
     <t>Task No</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>Get DSA Code of XMED from Niha's PC vah vah vah3</t>
+  </si>
+  <si>
+    <t>Get DSA Code of XMED from Niha's PC vah vah vivah 4</t>
   </si>
 </sst>
 </file>
@@ -776,8 +779,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H24" totalsRowShown="0">
-  <autoFilter ref="A1:H24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H25" totalsRowShown="0">
+  <autoFilter ref="A1:H25"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Task No"/>
     <tableColumn id="2" name="Task"/>
@@ -1055,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1631,6 +1634,29 @@
         <v>33</v>
       </c>
     </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>100</v>
+      </c>
+      <c r="E25" s="1">
+        <v>45727</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>